<commit_message>
Cambios a plantillas excel
</commit_message>
<xml_diff>
--- a/frontend/public/documents/plantillas/excel/Plantilla_Lista_Alumnos.xlsx
+++ b/frontend/public/documents/plantillas/excel/Plantilla_Lista_Alumnos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Documents\ServicioSocial\Indices\frontend\public\documents\plantillas\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACEB8D9-A848-49FB-A309-6FDA88562A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4759B629-BCEB-4A9A-8273-941966DFC184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{5A2D4DA5-1458-4BB9-AE11-E0C90FD3C75A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{5A2D4DA5-1458-4BB9-AE11-E0C90FD3C75A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,43 +34,55 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Numero de control</t>
-  </si>
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Apellido Paterno</t>
-  </si>
-  <si>
-    <t>Apellido Materno</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>CURP</t>
   </si>
   <si>
-    <t>Carrera actual</t>
+    <t>NO_CONTROL</t>
   </si>
   <si>
-    <t>Semestre</t>
+    <t>PATERNO</t>
   </si>
   <si>
-    <t>Ingreso</t>
+    <t>MATERNO</t>
   </si>
   <si>
-    <t>Periodo Ingreso</t>
+    <t>NOMBRE</t>
+  </si>
+  <si>
+    <t>CARRERA</t>
+  </si>
+  <si>
+    <t>PERIODO</t>
+  </si>
+  <si>
+    <t>(CAMBIAR EL TITULO DE LA COLUMNA PERIODO POR EL NUMERO DE PERIODO CORRESPONDIENTE)</t>
+  </si>
+  <si>
+    <t>LAS OPCIONES PARA LA COLUMNA PERIODO SON:</t>
+  </si>
+  <si>
+    <t>EXAMEN</t>
+  </si>
+  <si>
+    <t>EQUIVALENCIA</t>
+  </si>
+  <si>
+    <t>TRASLADO</t>
+  </si>
+  <si>
+    <t>REINGRESO</t>
+  </si>
+  <si>
+    <t>EN LA COLUMNA CARRERA UTILIZAR LA CLAVE DE LA CARRERA, NO EL NOMBRE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-yy"/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +91,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -147,44 +175,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="60% - Accent3" xfId="1" builtinId="40"/>
+    <cellStyle name="60% - Énfasis3" xfId="1" builtinId="40"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF1B396A"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="yyyy\-yy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -220,6 +239,15 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF1B396A"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -239,25 +267,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{19850345-1A1E-4E85-B5FA-5528F23902E9}" name="Table1" displayName="Table1" ref="A1:I1048576" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="11" tableBorderDxfId="10">
-  <autoFilter ref="A1:I1048576" xr:uid="{19850345-1A1E-4E85-B5FA-5528F23902E9}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{A4F8AF38-EBB9-47AD-83F7-487E1B19630C}" name="Numero de control" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{1D78E2CC-D977-42E3-ACAA-76CE02D499D4}" name="Nombre" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{B6F6F5DD-64AE-4F14-B1A2-F6BA7544902B}" name="Apellido Paterno" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{23BFD58F-9D9B-4107-9BE4-F423DCF7BF04}" name="Apellido Materno" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{2B0FC569-419C-4BF1-A439-7D86926E78B7}" name="CURP" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{2DC8E293-3471-40DE-88F0-9EF562B2DBCD}" name="Carrera actual" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{43BD6FA2-41A4-4103-A51A-403B276D4F40}" name="Semestre" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{D43D3537-78E0-4D75-90A4-65A9A46640F3}" name="Ingreso" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{B7B3D973-326B-40FB-8262-EA18363D4CD8}" name="Periodo Ingreso" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{19850345-1A1E-4E85-B5FA-5528F23902E9}" name="Table1" displayName="Table1" ref="A1:G1048576" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7">
+  <autoFilter ref="A1:G1048576" xr:uid="{19850345-1A1E-4E85-B5FA-5528F23902E9}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{A4F8AF38-EBB9-47AD-83F7-487E1B19630C}" name="CURP" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{1D78E2CC-D977-42E3-ACAA-76CE02D499D4}" name="NO_CONTROL" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{B6F6F5DD-64AE-4F14-B1A2-F6BA7544902B}" name="PATERNO" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{23BFD58F-9D9B-4107-9BE4-F423DCF7BF04}" name="MATERNO" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{2B0FC569-419C-4BF1-A439-7D86926E78B7}" name="NOMBRE" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{2DC8E293-3471-40DE-88F0-9EF562B2DBCD}" name="CARRERA" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{43BD6FA2-41A4-4103-A51A-403B276D4F40}" name="PERIODO" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -553,53 +579,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88AD4AF0-8E85-483B-A62E-805A8429A444}">
-  <dimension ref="A1:I124"/>
+  <dimension ref="A1:N124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="26" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="19" style="2" customWidth="1"/>
-    <col min="5" max="5" width="26.77734375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.77734375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="12.5546875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10" style="4" customWidth="1"/>
-    <col min="9" max="9" width="18.88671875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:14" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -607,10 +627,8 @@
       <c r="E2" s="1"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="5"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -618,10 +636,16 @@
       <c r="E3" s="1"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -629,10 +653,14 @@
       <c r="E4" s="1"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="5"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -640,21 +668,33 @@
       <c r="E5" s="1"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="C6" s="7"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="10"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -662,10 +702,16 @@
       <c r="E7" s="1"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="5"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="10"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -673,10 +719,16 @@
       <c r="E8" s="1"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I8" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="10"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -684,10 +736,16 @@
       <c r="E9" s="1"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="5"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="10"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -695,10 +753,14 @@
       <c r="E10" s="1"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -706,10 +768,16 @@
       <c r="E11" s="1"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="5"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -717,10 +785,14 @@
       <c r="E12" s="1"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -728,10 +800,8 @@
       <c r="E13" s="1"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="5"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -739,10 +809,8 @@
       <c r="E14" s="1"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -750,10 +818,8 @@
       <c r="E15" s="1"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -761,10 +827,8 @@
       <c r="E16" s="1"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="5"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -772,10 +836,8 @@
       <c r="E17" s="1"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="5"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -783,10 +845,8 @@
       <c r="E18" s="1"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="5"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -794,10 +854,8 @@
       <c r="E19" s="1"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="5"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -805,10 +863,8 @@
       <c r="E20" s="1"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="5"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -816,10 +872,8 @@
       <c r="E21" s="1"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="5"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -827,10 +881,8 @@
       <c r="E22" s="1"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="5"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -838,10 +890,8 @@
       <c r="E23" s="1"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="5"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -849,10 +899,8 @@
       <c r="E24" s="1"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="5"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -860,10 +908,8 @@
       <c r="E25" s="1"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="5"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -871,10 +917,8 @@
       <c r="E26" s="1"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="5"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -882,10 +926,8 @@
       <c r="E27" s="1"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="5"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -893,10 +935,8 @@
       <c r="E28" s="1"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="5"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -904,10 +944,8 @@
       <c r="E29" s="1"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="5"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -915,10 +953,8 @@
       <c r="E30" s="1"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="5"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -926,10 +962,8 @@
       <c r="E31" s="1"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="5"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -937,10 +971,8 @@
       <c r="E32" s="1"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="5"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -948,10 +980,8 @@
       <c r="E33" s="1"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="5"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -959,10 +989,8 @@
       <c r="E34" s="1"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="5"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -970,10 +998,8 @@
       <c r="E35" s="1"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="5"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -981,10 +1007,8 @@
       <c r="E36" s="1"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="5"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -992,10 +1016,8 @@
       <c r="E37" s="1"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="5"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1003,10 +1025,8 @@
       <c r="E38" s="1"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="5"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1014,10 +1034,8 @@
       <c r="E39" s="1"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="5"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1025,10 +1043,8 @@
       <c r="E40" s="1"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="5"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1036,10 +1052,8 @@
       <c r="E41" s="1"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="5"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1047,10 +1061,8 @@
       <c r="E42" s="1"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="5"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1058,10 +1070,8 @@
       <c r="E43" s="1"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="5"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1069,10 +1079,8 @@
       <c r="E44" s="1"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="5"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1080,10 +1088,8 @@
       <c r="E45" s="1"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="5"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1091,10 +1097,8 @@
       <c r="E46" s="1"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="5"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1102,10 +1106,8 @@
       <c r="E47" s="1"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="5"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1113,10 +1115,8 @@
       <c r="E48" s="1"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="5"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1124,10 +1124,8 @@
       <c r="E49" s="1"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="5"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1135,10 +1133,8 @@
       <c r="E50" s="1"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="5"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1146,10 +1142,8 @@
       <c r="E51" s="1"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="5"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1157,10 +1151,8 @@
       <c r="E52" s="1"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="5"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1168,10 +1160,8 @@
       <c r="E53" s="1"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="5"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1179,10 +1169,8 @@
       <c r="E54" s="1"/>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="5"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1190,10 +1178,8 @@
       <c r="E55" s="1"/>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="5"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1201,10 +1187,8 @@
       <c r="E56" s="1"/>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
-      <c r="I56" s="5"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1212,10 +1196,8 @@
       <c r="E57" s="1"/>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
-      <c r="H57" s="3"/>
-      <c r="I57" s="5"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1223,10 +1205,8 @@
       <c r="E58" s="1"/>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
-      <c r="H58" s="3"/>
-      <c r="I58" s="5"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1234,10 +1214,8 @@
       <c r="E59" s="1"/>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
-      <c r="H59" s="3"/>
-      <c r="I59" s="5"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1245,10 +1223,8 @@
       <c r="E60" s="1"/>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
-      <c r="H60" s="3"/>
-      <c r="I60" s="5"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1256,10 +1232,8 @@
       <c r="E61" s="1"/>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
-      <c r="H61" s="3"/>
-      <c r="I61" s="5"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1267,10 +1241,8 @@
       <c r="E62" s="1"/>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
-      <c r="H62" s="3"/>
-      <c r="I62" s="5"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1278,10 +1250,8 @@
       <c r="E63" s="1"/>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
-      <c r="H63" s="3"/>
-      <c r="I63" s="5"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1289,10 +1259,8 @@
       <c r="E64" s="1"/>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
-      <c r="H64" s="3"/>
-      <c r="I64" s="5"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1300,10 +1268,8 @@
       <c r="E65" s="1"/>
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
-      <c r="H65" s="3"/>
-      <c r="I65" s="5"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1311,10 +1277,8 @@
       <c r="E66" s="1"/>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
-      <c r="H66" s="3"/>
-      <c r="I66" s="5"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1322,10 +1286,8 @@
       <c r="E67" s="1"/>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
-      <c r="H67" s="3"/>
-      <c r="I67" s="5"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -1333,10 +1295,8 @@
       <c r="E68" s="1"/>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
-      <c r="H68" s="3"/>
-      <c r="I68" s="5"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -1344,10 +1304,8 @@
       <c r="E69" s="1"/>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
-      <c r="H69" s="3"/>
-      <c r="I69" s="5"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -1355,10 +1313,8 @@
       <c r="E70" s="1"/>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
-      <c r="H70" s="3"/>
-      <c r="I70" s="5"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -1366,10 +1322,8 @@
       <c r="E71" s="1"/>
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
-      <c r="H71" s="3"/>
-      <c r="I71" s="5"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -1377,10 +1331,8 @@
       <c r="E72" s="1"/>
       <c r="F72" s="3"/>
       <c r="G72" s="3"/>
-      <c r="H72" s="3"/>
-      <c r="I72" s="5"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -1388,10 +1340,8 @@
       <c r="E73" s="1"/>
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
-      <c r="H73" s="3"/>
-      <c r="I73" s="5"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -1399,10 +1349,8 @@
       <c r="E74" s="1"/>
       <c r="F74" s="3"/>
       <c r="G74" s="3"/>
-      <c r="H74" s="3"/>
-      <c r="I74" s="5"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -1410,10 +1358,8 @@
       <c r="E75" s="1"/>
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
-      <c r="H75" s="3"/>
-      <c r="I75" s="5"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -1421,10 +1367,8 @@
       <c r="E76" s="1"/>
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
-      <c r="H76" s="3"/>
-      <c r="I76" s="5"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -1432,10 +1376,8 @@
       <c r="E77" s="1"/>
       <c r="F77" s="3"/>
       <c r="G77" s="3"/>
-      <c r="H77" s="3"/>
-      <c r="I77" s="5"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -1443,10 +1385,8 @@
       <c r="E78" s="1"/>
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
-      <c r="H78" s="3"/>
-      <c r="I78" s="5"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -1454,10 +1394,8 @@
       <c r="E79" s="1"/>
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
-      <c r="H79" s="3"/>
-      <c r="I79" s="5"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -1465,10 +1403,8 @@
       <c r="E80" s="1"/>
       <c r="F80" s="3"/>
       <c r="G80" s="3"/>
-      <c r="H80" s="3"/>
-      <c r="I80" s="5"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -1476,10 +1412,8 @@
       <c r="E81" s="1"/>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
-      <c r="H81" s="3"/>
-      <c r="I81" s="5"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -1487,10 +1421,8 @@
       <c r="E82" s="1"/>
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
-      <c r="H82" s="3"/>
-      <c r="I82" s="5"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -1498,10 +1430,8 @@
       <c r="E83" s="1"/>
       <c r="F83" s="3"/>
       <c r="G83" s="3"/>
-      <c r="H83" s="3"/>
-      <c r="I83" s="5"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -1509,10 +1439,8 @@
       <c r="E84" s="1"/>
       <c r="F84" s="3"/>
       <c r="G84" s="3"/>
-      <c r="H84" s="3"/>
-      <c r="I84" s="5"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -1520,10 +1448,8 @@
       <c r="E85" s="1"/>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
-      <c r="H85" s="3"/>
-      <c r="I85" s="5"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -1531,10 +1457,8 @@
       <c r="E86" s="1"/>
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
-      <c r="H86" s="3"/>
-      <c r="I86" s="5"/>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -1542,10 +1466,8 @@
       <c r="E87" s="1"/>
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
-      <c r="H87" s="3"/>
-      <c r="I87" s="5"/>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -1553,10 +1475,8 @@
       <c r="E88" s="1"/>
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
-      <c r="H88" s="3"/>
-      <c r="I88" s="5"/>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -1564,10 +1484,8 @@
       <c r="E89" s="1"/>
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
-      <c r="H89" s="3"/>
-      <c r="I89" s="5"/>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -1575,10 +1493,8 @@
       <c r="E90" s="1"/>
       <c r="F90" s="3"/>
       <c r="G90" s="3"/>
-      <c r="H90" s="3"/>
-      <c r="I90" s="5"/>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -1586,10 +1502,8 @@
       <c r="E91" s="1"/>
       <c r="F91" s="3"/>
       <c r="G91" s="3"/>
-      <c r="H91" s="3"/>
-      <c r="I91" s="5"/>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -1597,10 +1511,8 @@
       <c r="E92" s="1"/>
       <c r="F92" s="3"/>
       <c r="G92" s="3"/>
-      <c r="H92" s="3"/>
-      <c r="I92" s="5"/>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -1608,10 +1520,8 @@
       <c r="E93" s="1"/>
       <c r="F93" s="3"/>
       <c r="G93" s="3"/>
-      <c r="H93" s="3"/>
-      <c r="I93" s="5"/>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -1619,10 +1529,8 @@
       <c r="E94" s="1"/>
       <c r="F94" s="3"/>
       <c r="G94" s="3"/>
-      <c r="H94" s="3"/>
-      <c r="I94" s="5"/>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -1630,10 +1538,8 @@
       <c r="E95" s="1"/>
       <c r="F95" s="3"/>
       <c r="G95" s="3"/>
-      <c r="H95" s="3"/>
-      <c r="I95" s="5"/>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -1641,10 +1547,8 @@
       <c r="E96" s="1"/>
       <c r="F96" s="3"/>
       <c r="G96" s="3"/>
-      <c r="H96" s="3"/>
-      <c r="I96" s="5"/>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -1652,10 +1556,8 @@
       <c r="E97" s="1"/>
       <c r="F97" s="3"/>
       <c r="G97" s="3"/>
-      <c r="H97" s="3"/>
-      <c r="I97" s="5"/>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -1663,10 +1565,8 @@
       <c r="E98" s="1"/>
       <c r="F98" s="3"/>
       <c r="G98" s="3"/>
-      <c r="H98" s="3"/>
-      <c r="I98" s="5"/>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -1674,10 +1574,8 @@
       <c r="E99" s="1"/>
       <c r="F99" s="3"/>
       <c r="G99" s="3"/>
-      <c r="H99" s="3"/>
-      <c r="I99" s="5"/>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -1685,10 +1583,8 @@
       <c r="E100" s="1"/>
       <c r="F100" s="3"/>
       <c r="G100" s="3"/>
-      <c r="H100" s="3"/>
-      <c r="I100" s="5"/>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -1696,10 +1592,8 @@
       <c r="E101" s="1"/>
       <c r="F101" s="3"/>
       <c r="G101" s="3"/>
-      <c r="H101" s="3"/>
-      <c r="I101" s="5"/>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -1707,10 +1601,8 @@
       <c r="E102" s="1"/>
       <c r="F102" s="3"/>
       <c r="G102" s="3"/>
-      <c r="H102" s="3"/>
-      <c r="I102" s="5"/>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -1718,10 +1610,8 @@
       <c r="E103" s="1"/>
       <c r="F103" s="3"/>
       <c r="G103" s="3"/>
-      <c r="H103" s="3"/>
-      <c r="I103" s="5"/>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -1729,10 +1619,8 @@
       <c r="E104" s="1"/>
       <c r="F104" s="3"/>
       <c r="G104" s="3"/>
-      <c r="H104" s="3"/>
-      <c r="I104" s="5"/>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -1740,10 +1628,8 @@
       <c r="E105" s="1"/>
       <c r="F105" s="3"/>
       <c r="G105" s="3"/>
-      <c r="H105" s="3"/>
-      <c r="I105" s="5"/>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -1751,10 +1637,8 @@
       <c r="E106" s="1"/>
       <c r="F106" s="3"/>
       <c r="G106" s="3"/>
-      <c r="H106" s="3"/>
-      <c r="I106" s="5"/>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -1762,10 +1646,8 @@
       <c r="E107" s="1"/>
       <c r="F107" s="3"/>
       <c r="G107" s="3"/>
-      <c r="H107" s="3"/>
-      <c r="I107" s="5"/>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -1773,10 +1655,8 @@
       <c r="E108" s="1"/>
       <c r="F108" s="3"/>
       <c r="G108" s="3"/>
-      <c r="H108" s="3"/>
-      <c r="I108" s="5"/>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -1784,10 +1664,8 @@
       <c r="E109" s="1"/>
       <c r="F109" s="3"/>
       <c r="G109" s="3"/>
-      <c r="H109" s="3"/>
-      <c r="I109" s="5"/>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -1795,10 +1673,8 @@
       <c r="E110" s="1"/>
       <c r="F110" s="3"/>
       <c r="G110" s="3"/>
-      <c r="H110" s="3"/>
-      <c r="I110" s="5"/>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -1806,10 +1682,8 @@
       <c r="E111" s="1"/>
       <c r="F111" s="3"/>
       <c r="G111" s="3"/>
-      <c r="H111" s="3"/>
-      <c r="I111" s="5"/>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -1817,10 +1691,8 @@
       <c r="E112" s="1"/>
       <c r="F112" s="3"/>
       <c r="G112" s="3"/>
-      <c r="H112" s="3"/>
-      <c r="I112" s="5"/>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -1828,10 +1700,8 @@
       <c r="E113" s="1"/>
       <c r="F113" s="3"/>
       <c r="G113" s="3"/>
-      <c r="H113" s="3"/>
-      <c r="I113" s="5"/>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -1839,10 +1709,8 @@
       <c r="E114" s="1"/>
       <c r="F114" s="3"/>
       <c r="G114" s="3"/>
-      <c r="H114" s="3"/>
-      <c r="I114" s="5"/>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -1850,10 +1718,8 @@
       <c r="E115" s="1"/>
       <c r="F115" s="3"/>
       <c r="G115" s="3"/>
-      <c r="H115" s="3"/>
-      <c r="I115" s="5"/>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -1861,10 +1727,8 @@
       <c r="E116" s="1"/>
       <c r="F116" s="3"/>
       <c r="G116" s="3"/>
-      <c r="H116" s="3"/>
-      <c r="I116" s="5"/>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -1872,10 +1736,8 @@
       <c r="E117" s="1"/>
       <c r="F117" s="3"/>
       <c r="G117" s="3"/>
-      <c r="H117" s="3"/>
-      <c r="I117" s="5"/>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -1883,10 +1745,8 @@
       <c r="E118" s="1"/>
       <c r="F118" s="3"/>
       <c r="G118" s="3"/>
-      <c r="H118" s="3"/>
-      <c r="I118" s="5"/>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -1894,10 +1754,8 @@
       <c r="E119" s="1"/>
       <c r="F119" s="3"/>
       <c r="G119" s="3"/>
-      <c r="H119" s="3"/>
-      <c r="I119" s="5"/>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -1905,10 +1763,8 @@
       <c r="E120" s="1"/>
       <c r="F120" s="3"/>
       <c r="G120" s="3"/>
-      <c r="H120" s="3"/>
-      <c r="I120" s="5"/>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -1916,10 +1772,8 @@
       <c r="E121" s="1"/>
       <c r="F121" s="3"/>
       <c r="G121" s="3"/>
-      <c r="H121" s="3"/>
-      <c r="I121" s="5"/>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -1927,10 +1781,8 @@
       <c r="E122" s="1"/>
       <c r="F122" s="3"/>
       <c r="G122" s="3"/>
-      <c r="H122" s="3"/>
-      <c r="I122" s="5"/>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -1938,10 +1790,8 @@
       <c r="E123" s="1"/>
       <c r="F123" s="3"/>
       <c r="G123" s="3"/>
-      <c r="H123" s="3"/>
-      <c r="I123" s="5"/>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -1949,34 +1799,19 @@
       <c r="E124" s="1"/>
       <c r="F124" s="3"/>
       <c r="G124" s="3"/>
-      <c r="H124" s="3"/>
-      <c r="I124" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="5">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{321749E7-15BA-4554-B9A3-58856F036700}">
-      <formula1>1</formula1>
-      <formula2>4</formula2>
-    </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{B03FFF67-BE64-4865-8792-58FE6BE11D6F}">
-      <formula1>1</formula1>
-      <formula2>20</formula2>
-    </dataValidation>
-    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{8D3A86A5-C2D7-4DA8-8D63-6974FA1DA653}">
-      <formula1>18</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{2E1B9AAE-8416-4521-9239-C7C9BE1523CF}">
-      <formula1>12</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I1048576" xr:uid="{AB412D3F-0D5D-407E-9755-1610F549609C}">
-      <formula1>6</formula1>
-    </dataValidation>
-  </dataValidations>
+  <mergeCells count="7">
+    <mergeCell ref="I11:N12"/>
+    <mergeCell ref="I3:N4"/>
+    <mergeCell ref="I5:N5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="A1 H1:I1 F1" listDataValidation="1"/>
-  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>